<commit_message>
Added csv to fietssimulatie
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94DE10E-175F-4EFF-A272-0098FB5F3968}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7170418A-114F-4A4D-B965-6DE4E9CE567D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Dag</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Coderen Fietssimulatie (onzeker van formules)</t>
+  </si>
+  <si>
+    <t>Coderen fietssimulatie</t>
   </si>
 </sst>
 </file>
@@ -374,10 +377,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +404,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2:B99)</f>
-        <v>8</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -479,6 +482,17 @@
       </c>
       <c r="C8" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43381</v>
+      </c>
+      <c r="B9">
+        <v>0.75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Fload + variable t_dc
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7170418A-114F-4A4D-B965-6DE4E9CE567D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D15361D-5966-4B64-8602-E55ACAC93B02}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Dag</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Coderen fietssimulatie</t>
+  </si>
+  <si>
+    <t>Coderen fietssimulatie drag + timeslots</t>
+  </si>
+  <si>
+    <t>Keras/TF werkende krijgen</t>
+  </si>
+  <si>
+    <t>Keras bekijken/leren</t>
   </si>
 </sst>
 </file>
@@ -377,10 +386,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +413,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2:B99)</f>
-        <v>8.75</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -493,6 +502,50 @@
       </c>
       <c r="C9" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43382</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43386</v>
+      </c>
+      <c r="B11">
+        <v>1.5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43387</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43387</v>
+      </c>
+      <c r="B13">
+        <v>1.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simulation updated with variable t_dc and slope generation + start learning (lstm)
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9419C2F-686D-4527-926B-954ABFD93911}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928D2E01-E090-4476-8AD2-47667887DA6F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Dag</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Literatuur studie</t>
+  </si>
+  <si>
+    <t>Fietssimulatie bijwerken</t>
+  </si>
+  <si>
+    <t>Preprocessing</t>
   </si>
 </sst>
 </file>
@@ -398,10 +404,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +431,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2:B99)</f>
-        <v>22.75</v>
+        <v>29.75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -613,6 +619,51 @@
       </c>
       <c r="C18" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43399</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43404</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43406</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="str">
+        <f>C20</f>
+        <v>Fietssimulatie bijwerken</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43407</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added classification + simulation tweeks
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF19FF33-D1AA-4AA9-B768-7F538FFE3367}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001CD79B-5666-4BC3-BF84-1408BDAA2122}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Dag</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Literatuurstudie (Passive aggressive algorithm)</t>
+  </si>
+  <si>
+    <t>In order brengen fietssimulatie + classificatie toevoegen</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +446,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2:B99)</f>
-        <v>43.75</v>
+        <v>46.75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -731,6 +734,28 @@
       </c>
       <c r="C27" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43419</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43421</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>